<commit_message>
Created Award Group Files for Experiment. Created a file in R to run the imports.
</commit_message>
<xml_diff>
--- a/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
+++ b/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$22</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TotalApplicationsForAwardingGroup</t>
   </si>
@@ -40,6 +43,9 @@
   </si>
   <si>
     <t>AwardingGroupId</t>
+  </si>
+  <si>
+    <t>Rankable</t>
   </si>
 </sst>
 </file>
@@ -92,6 +98,2410 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Max vs Min Applicant Awards</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MaxAward</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10860</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6005.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2333.33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>12548</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-295F-4A23-AFC9-291B5A8E38D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MinAward</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>415.54</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3750</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2548</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-295F-4A23-AFC9-291B5A8E38D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="673889584"/>
+        <c:axId val="673890240"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="673889584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="673890240"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="673890240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="673889584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Awards</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Unique Awardees</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DistinctAwards</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>663</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>306</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F017-4591-86BF-90FE89E3C1C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>DistinctAwardees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>482</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>361</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F017-4591-86BF-90FE89E3C1C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="672386152"/>
+        <c:axId val="672382544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="672386152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672382544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="672382544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="672386152"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1357312</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>976312</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,10 +2767,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,7 +2784,7 @@
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -396,8 +2806,11 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -419,8 +2832,11 @@
       <c r="G2">
         <v>226</v>
       </c>
+      <c r="H2">
+        <v>4121</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -442,8 +2858,11 @@
       <c r="G3">
         <v>0</v>
       </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -465,8 +2884,11 @@
       <c r="G4">
         <v>157</v>
       </c>
+      <c r="H4">
+        <v>23065</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -488,8 +2910,11 @@
       <c r="G5">
         <v>500</v>
       </c>
+      <c r="H5">
+        <v>57</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -511,8 +2936,11 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -534,8 +2962,11 @@
       <c r="G7">
         <v>480</v>
       </c>
+      <c r="H7">
+        <v>538</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -557,8 +2988,11 @@
       <c r="G8">
         <v>100</v>
       </c>
+      <c r="H8">
+        <v>15779</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -580,8 +3014,11 @@
       <c r="G9">
         <v>0</v>
       </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -603,8 +3040,11 @@
       <c r="G10">
         <v>600</v>
       </c>
+      <c r="H10">
+        <v>3505</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -626,8 +3066,11 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11">
+        <v>122</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -649,8 +3092,11 @@
       <c r="G12">
         <v>500</v>
       </c>
+      <c r="H12">
+        <v>110</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -672,8 +3118,11 @@
       <c r="G13">
         <v>400</v>
       </c>
+      <c r="H13">
+        <v>991</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -695,8 +3144,11 @@
       <c r="G14">
         <v>415.54</v>
       </c>
+      <c r="H14">
+        <v>440</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -718,8 +3170,11 @@
       <c r="G15">
         <v>3750</v>
       </c>
+      <c r="H15">
+        <v>61</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -741,8 +3196,11 @@
       <c r="G16">
         <v>0</v>
       </c>
+      <c r="H16">
+        <v>9828</v>
+      </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -764,8 +3222,11 @@
       <c r="G17">
         <v>2548</v>
       </c>
+      <c r="H17">
+        <v>4226</v>
+      </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -787,8 +3248,11 @@
       <c r="G18">
         <v>0</v>
       </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -810,8 +3274,11 @@
       <c r="G19">
         <v>333</v>
       </c>
+      <c r="H19">
+        <v>302</v>
+      </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -833,8 +3300,11 @@
       <c r="G20">
         <v>0</v>
       </c>
+      <c r="H20">
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -856,8 +3326,11 @@
       <c r="G21">
         <v>0</v>
       </c>
+      <c r="H21">
+        <v>120</v>
+      </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -878,9 +3351,13 @@
       </c>
       <c r="G22">
         <v>1000</v>
+      </c>
+      <c r="H22">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished experiment and conclusion.
</commit_message>
<xml_diff>
--- a/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
+++ b/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
@@ -5,24 +5,26 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Documents\scholarshipawardingprocess\Experiment Parts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\ScholarshipAwardingProcess\scholarshipawardingprocess\Experiment Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Results" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
   <si>
     <t>TotalApplicationsForAwardingGroup</t>
   </si>
@@ -47,18 +49,57 @@
   <si>
     <t>Rankable</t>
   </si>
+  <si>
+    <t>Top Algo</t>
+  </si>
+  <si>
+    <t>RA1</t>
+  </si>
+  <si>
+    <t>RA2</t>
+  </si>
+  <si>
+    <t>RA3</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Unique</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>1   1   1               1              1         500.00          500.00</t>
+  </si>
+  <si>
+    <t>0   0             302            193       10428.86            62.5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2769,8 +2813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3360,4 +3404,1386 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>6995</v>
+      </c>
+      <c r="C2">
+        <v>505</v>
+      </c>
+      <c r="D2">
+        <v>275</v>
+      </c>
+      <c r="E2">
+        <v>211</v>
+      </c>
+      <c r="F2">
+        <v>10000</v>
+      </c>
+      <c r="G2">
+        <v>226</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>4121</v>
+      </c>
+      <c r="M2">
+        <v>364</v>
+      </c>
+      <c r="N2">
+        <v>28632.959999999999</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>3548</v>
+      </c>
+      <c r="C3">
+        <v>67</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>46785</v>
+      </c>
+      <c r="C4">
+        <v>3437</v>
+      </c>
+      <c r="D4">
+        <v>421</v>
+      </c>
+      <c r="E4">
+        <v>397</v>
+      </c>
+      <c r="F4">
+        <v>10860</v>
+      </c>
+      <c r="G4">
+        <v>157</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>23065</v>
+      </c>
+      <c r="M4">
+        <v>1773</v>
+      </c>
+      <c r="N4">
+        <v>105269.9</v>
+      </c>
+      <c r="O4">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>322</v>
+      </c>
+      <c r="C5">
+        <v>264</v>
+      </c>
+      <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>2000</v>
+      </c>
+      <c r="G5">
+        <v>500</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>53</v>
+      </c>
+      <c r="M5">
+        <v>42</v>
+      </c>
+      <c r="N5">
+        <v>1771.74</v>
+      </c>
+      <c r="O5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>900</v>
+      </c>
+      <c r="C7">
+        <v>355</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>61</v>
+      </c>
+      <c r="F7">
+        <v>10000</v>
+      </c>
+      <c r="G7">
+        <v>480</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>538</v>
+      </c>
+      <c r="M7">
+        <v>234</v>
+      </c>
+      <c r="N7">
+        <v>8153.92</v>
+      </c>
+      <c r="O7">
+        <v>13.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>24983</v>
+      </c>
+      <c r="C8">
+        <v>824</v>
+      </c>
+      <c r="D8">
+        <v>663</v>
+      </c>
+      <c r="E8">
+        <v>482</v>
+      </c>
+      <c r="F8">
+        <v>17000</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>15779</v>
+      </c>
+      <c r="M8">
+        <v>556</v>
+      </c>
+      <c r="N8">
+        <v>28783.39</v>
+      </c>
+      <c r="O8">
+        <v>12.54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>230</v>
+      </c>
+      <c r="C9">
+        <v>224</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4547</v>
+      </c>
+      <c r="C10">
+        <v>350</v>
+      </c>
+      <c r="D10">
+        <v>306</v>
+      </c>
+      <c r="E10">
+        <v>226</v>
+      </c>
+      <c r="F10">
+        <v>6005.2</v>
+      </c>
+      <c r="G10">
+        <v>600</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>3505</v>
+      </c>
+      <c r="M10">
+        <v>261</v>
+      </c>
+      <c r="N10">
+        <v>6671.32</v>
+      </c>
+      <c r="O10">
+        <v>254.81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>30000</v>
+      </c>
+      <c r="O11">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>112</v>
+      </c>
+      <c r="C12">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>15</v>
+      </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>5000</v>
+      </c>
+      <c r="G12">
+        <v>500</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>110</v>
+      </c>
+      <c r="M12">
+        <v>28</v>
+      </c>
+      <c r="N12">
+        <v>1899.05</v>
+      </c>
+      <c r="O12">
+        <v>105.26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1114</v>
+      </c>
+      <c r="C13">
+        <v>127</v>
+      </c>
+      <c r="D13">
+        <v>79</v>
+      </c>
+      <c r="E13">
+        <v>56</v>
+      </c>
+      <c r="F13">
+        <v>8800</v>
+      </c>
+      <c r="G13">
+        <v>400</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>991</v>
+      </c>
+      <c r="M13">
+        <v>112</v>
+      </c>
+      <c r="N13">
+        <v>4204.96</v>
+      </c>
+      <c r="O13">
+        <v>16.13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>534</v>
+      </c>
+      <c r="C14">
+        <v>121</v>
+      </c>
+      <c r="D14">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>52</v>
+      </c>
+      <c r="F14">
+        <v>2333.33</v>
+      </c>
+      <c r="G14">
+        <v>415.54</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>440</v>
+      </c>
+      <c r="M14">
+        <v>97</v>
+      </c>
+      <c r="N14">
+        <v>3609.75</v>
+      </c>
+      <c r="O14">
+        <v>116.67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>3750</v>
+      </c>
+      <c r="G15">
+        <v>3750</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
+        <v>31200</v>
+      </c>
+      <c r="O15">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>17410</v>
+      </c>
+      <c r="C16">
+        <v>358</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>9828</v>
+      </c>
+      <c r="M16">
+        <v>211</v>
+      </c>
+      <c r="N16">
+        <v>10827.37</v>
+      </c>
+      <c r="O16">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>4886</v>
+      </c>
+      <c r="C17">
+        <v>376</v>
+      </c>
+      <c r="D17">
+        <v>460</v>
+      </c>
+      <c r="E17">
+        <v>361</v>
+      </c>
+      <c r="F17">
+        <v>12548</v>
+      </c>
+      <c r="G17">
+        <v>2548</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>4226</v>
+      </c>
+      <c r="M17">
+        <v>305</v>
+      </c>
+      <c r="N17">
+        <v>6464.05</v>
+      </c>
+      <c r="O17">
+        <v>158.76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>175</v>
+      </c>
+      <c r="C18">
+        <v>51</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" t="s">
+        <v>18</v>
+      </c>
+      <c r="O18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1503</v>
+      </c>
+      <c r="C19">
+        <v>1064</v>
+      </c>
+      <c r="D19">
+        <v>92</v>
+      </c>
+      <c r="E19">
+        <v>91</v>
+      </c>
+      <c r="F19">
+        <v>5000</v>
+      </c>
+      <c r="G19">
+        <v>333</v>
+      </c>
+      <c r="H19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>302</v>
+      </c>
+      <c r="M19">
+        <v>193</v>
+      </c>
+      <c r="N19">
+        <v>10428.86</v>
+      </c>
+      <c r="O19">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>500</v>
+      </c>
+      <c r="O20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+      <c r="C21">
+        <v>104</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>3</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+      <c r="N21">
+        <v>20000</v>
+      </c>
+      <c r="O21">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1000</v>
+      </c>
+      <c r="G22">
+        <v>1000</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1000</v>
+      </c>
+      <c r="O22">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>275</v>
+      </c>
+      <c r="C2">
+        <v>211</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>421</v>
+      </c>
+      <c r="C3">
+        <v>397</v>
+      </c>
+      <c r="D3">
+        <v>10860</v>
+      </c>
+      <c r="E3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>61</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>663</v>
+      </c>
+      <c r="C6">
+        <v>482</v>
+      </c>
+      <c r="D6">
+        <v>17000</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>306</v>
+      </c>
+      <c r="C7">
+        <v>226</v>
+      </c>
+      <c r="D7">
+        <v>6005.2</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>5000</v>
+      </c>
+      <c r="E8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>79</v>
+      </c>
+      <c r="C9">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>8800</v>
+      </c>
+      <c r="E9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>63</v>
+      </c>
+      <c r="C10">
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <v>2333.33</v>
+      </c>
+      <c r="E10">
+        <v>415.54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>3750</v>
+      </c>
+      <c r="E11">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>460</v>
+      </c>
+      <c r="C12">
+        <v>361</v>
+      </c>
+      <c r="D12">
+        <v>12548</v>
+      </c>
+      <c r="E12">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>92</v>
+      </c>
+      <c r="C13">
+        <v>91</v>
+      </c>
+      <c r="D13">
+        <v>5000</v>
+      </c>
+      <c r="E13">
+        <v>333</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <v>20000</v>
+      </c>
+      <c r="M15">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1000</v>
+      </c>
+      <c r="E16">
+        <v>1000</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1000</v>
+      </c>
+      <c r="M16">
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some charts for rankings. Needed to tweak the paper just a little with new view of data.
</commit_message>
<xml_diff>
--- a/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
+++ b/Experiment Parts/AwardingGroupAwardingYear25Stats.xlsx
@@ -9,22 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Results" sheetId="2" r:id="rId3"/>
+    <sheet name="Just Rankable" sheetId="1" r:id="rId1"/>
+    <sheet name="Experiment Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Ranking Results" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Just Rankable'!$A$1:$H$22</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>TotalApplicationsForAwardingGroup</t>
   </si>
@@ -74,13 +74,43 @@
     <t>Min</t>
   </si>
   <si>
-    <t>1   1   1               1              1         500.00          500.00</t>
+    <t>x</t>
   </si>
   <si>
-    <t>0   0             302            193       10428.86            62.5</t>
+    <t>AlgorithmId</t>
   </si>
   <si>
-    <t>x</t>
+    <t>avgRank</t>
+  </si>
+  <si>
+    <t>cntOf1stRanked</t>
+  </si>
+  <si>
+    <t>2nd Ranked</t>
+  </si>
+  <si>
+    <t>3rd Ranking</t>
+  </si>
+  <si>
+    <t>1st Ranked</t>
+  </si>
+  <si>
+    <t>4th Ranked</t>
+  </si>
+  <si>
+    <t>5th Ranked</t>
+  </si>
+  <si>
+    <t>6th Ranked</t>
+  </si>
+  <si>
+    <t>7th Ranked</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -122,10 +152,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -184,7 +220,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -226,7 +261,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>'Just Rankable'!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -247,7 +282,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>'Just Rankable'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -319,7 +354,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$22</c:f>
+              <c:f>'Just Rankable'!$F$2:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -400,7 +435,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>'Just Rankable'!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -421,7 +456,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>'Just Rankable'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -493,7 +528,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$22</c:f>
+              <c:f>'Just Rankable'!$G$2:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -699,7 +734,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -811,7 +845,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -853,7 +886,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>'Just Rankable'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -874,7 +907,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>'Just Rankable'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -946,7 +979,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$22</c:f>
+              <c:f>'Just Rankable'!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1027,7 +1060,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>'Just Rankable'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1048,7 +1081,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$22</c:f>
+              <c:f>'Just Rankable'!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1120,7 +1153,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$22</c:f>
+              <c:f>'Just Rankable'!$E$2:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
@@ -1326,7 +1359,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3410,7 +3442,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -3533,7 +3565,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3653,28 +3685,28 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -3794,28 +3826,28 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -4217,28 +4249,28 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="N18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
@@ -4436,350 +4468,616 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:M1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2.1764700000000001</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>11</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>3.1176469999999998</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="L4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4.5882350000000001</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>5.1176469999999998</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>6</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G14" s="1"/>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2">
+        <v>4</v>
+      </c>
+      <c r="N16" s="2">
+        <v>5</v>
+      </c>
+      <c r="O16" s="2">
+        <v>6</v>
+      </c>
+      <c r="P16" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>5.1176469999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
+        <v>2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>5</v>
+      </c>
+      <c r="O18" s="2">
+        <v>5</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>4.5882350000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>2</v>
+      </c>
+      <c r="M19" s="2">
+        <v>2</v>
+      </c>
+      <c r="N19" s="2">
+        <v>7</v>
+      </c>
+      <c r="O19" s="2">
+        <v>6</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>8</v>
+      </c>
+      <c r="M20" s="2">
+        <v>4</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="2">
+        <v>11</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2">
+        <v>2</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2</v>
+      </c>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>2.1764700000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I22" s="2">
+        <v>6</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
+      <c r="L22" s="2">
+        <v>5</v>
+      </c>
+      <c r="M22" s="2">
+        <v>8</v>
+      </c>
+      <c r="N22" s="2">
+        <v>0</v>
+      </c>
+      <c r="O22" s="2">
+        <v>2</v>
+      </c>
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I23" s="2">
+        <v>7</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>11</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2">
+        <v>0</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>3.1176469999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>7</v>
+      </c>
+      <c r="D26">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>275</v>
-      </c>
-      <c r="C2">
-        <v>211</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>421</v>
-      </c>
-      <c r="C3">
-        <v>397</v>
-      </c>
-      <c r="D3">
-        <v>10860</v>
-      </c>
-      <c r="E3">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4">
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>2000</v>
-      </c>
-      <c r="E4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>90</v>
-      </c>
-      <c r="C5">
-        <v>61</v>
-      </c>
-      <c r="D5">
-        <v>10000</v>
-      </c>
-      <c r="E5">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>663</v>
-      </c>
-      <c r="C6">
-        <v>482</v>
-      </c>
-      <c r="D6">
-        <v>17000</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>306</v>
-      </c>
-      <c r="C7">
-        <v>226</v>
-      </c>
-      <c r="D7">
-        <v>6005.2</v>
-      </c>
-      <c r="E7">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>15</v>
-      </c>
-      <c r="C8">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>5000</v>
-      </c>
-      <c r="E8">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>79</v>
-      </c>
-      <c r="C9">
-        <v>56</v>
-      </c>
-      <c r="D9">
-        <v>8800</v>
-      </c>
-      <c r="E9">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>63</v>
-      </c>
-      <c r="C10">
-        <v>52</v>
-      </c>
-      <c r="D10">
-        <v>2333.33</v>
-      </c>
-      <c r="E10">
-        <v>415.54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>14</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>3750</v>
-      </c>
-      <c r="E11">
-        <v>3750</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>16</v>
-      </c>
-      <c r="B12">
-        <v>460</v>
-      </c>
-      <c r="C12">
-        <v>361</v>
-      </c>
-      <c r="D12">
-        <v>12548</v>
-      </c>
-      <c r="E12">
-        <v>2548</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>92</v>
-      </c>
-      <c r="C13">
-        <v>91</v>
-      </c>
-      <c r="D13">
-        <v>5000</v>
-      </c>
-      <c r="E13">
-        <v>333</v>
-      </c>
-      <c r="F13">
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29">
         <v>5</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>19</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>3</v>
-      </c>
-      <c r="K15">
-        <v>2</v>
-      </c>
-      <c r="L15">
-        <v>20000</v>
-      </c>
-      <c r="M15">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>21</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>1000</v>
-      </c>
-      <c r="E16">
-        <v>1000</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1000</v>
-      </c>
-      <c r="M16">
-        <v>1000</v>
+      <c r="D29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>